<commit_message>
added technical indicators input and config
</commit_message>
<xml_diff>
--- a/server/technical-indicators-info.xlsx
+++ b/server/technical-indicators-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bb5771db89f4b71/Desktop/UNI/Fourth year/Dissertation/Repo/ATPlatform/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40C82BBD-ECCF-4B81-8A0C-E8C14A058AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{40C82BBD-ECCF-4B81-8A0C-E8C14A058AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D0AC1AC1-2CF4-4418-ACD1-8B1B96A80AAC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07D8F586-ED62-4F25-AB07-0DF1C28F4F51}"/>
+    <workbookView xWindow="13308" yWindow="3240" windowWidth="14352" windowHeight="11328" xr2:uid="{07D8F586-ED62-4F25-AB07-0DF1C28F4F51}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>Technical Indicators</t>
   </si>
@@ -168,21 +168,12 @@
     <t>signalPeriod</t>
   </si>
   <si>
-    <t>SimpleMAOscillator, SimpleMASignal</t>
-  </si>
-  <si>
     <t>[{ MACD, histogram, signal}]</t>
   </si>
   <si>
-    <t>step, max</t>
-  </si>
-  <si>
     <t>[{d,k}]</t>
   </si>
   <si>
-    <t>dPeriod, kPeriod, rsiPeriod, stochasticPeriod</t>
-  </si>
-  <si>
     <t>TO CHECK</t>
   </si>
   <si>
@@ -199,13 +190,46 @@
   </si>
   <si>
     <t>ROCPer1, ROCPer2, ROCPer3, ROCPer4, SMAROCPer1, SMAROCPer2, SMAROCPer3, SMAROCPer4</t>
+  </si>
+  <si>
+    <t>CONFIG DATA</t>
+  </si>
+  <si>
+    <t>DYNAMIC DATA</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>SimpleMAOscillator</t>
+  </si>
+  <si>
+    <t>SimpleMASignal</t>
+  </si>
+  <si>
+    <t>dPeriod</t>
+  </si>
+  <si>
+    <t>kPeriod</t>
+  </si>
+  <si>
+    <t>rsiPeriod</t>
+  </si>
+  <si>
+    <t>stochasticPeriod</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,8 +261,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,8 +295,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -266,12 +316,64 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
@@ -293,14 +395,119 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -321,22 +528,6 @@
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -351,10 +542,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD8B65D1-0B2E-41E6-BACF-5EB3D48F7370}" name="Tabella1" displayName="Tabella1" ref="A2:N28" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A2:N28" xr:uid="{ED24963E-54D4-4975-A2B7-5702B9FD8949}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{04C6B4C8-8C1B-4A37-9AC1-6BF23B0F893B}" name="Technical Indicators" dataDxfId="0" dataCellStyle="Collegamento ipertestuale"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD8B65D1-0B2E-41E6-BACF-5EB3D48F7370}" name="Tabella1" displayName="Tabella1" ref="A3:W29" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
+  <autoFilter ref="A3:W29" xr:uid="{ED24963E-54D4-4975-A2B7-5702B9FD8949}"/>
+  <tableColumns count="23">
+    <tableColumn id="1" xr3:uid="{04C6B4C8-8C1B-4A37-9AC1-6BF23B0F893B}" name="Technical Indicators" dataDxfId="9" dataCellStyle="Collegamento ipertestuale"/>
     <tableColumn id="2" xr3:uid="{03EB3258-1D12-4FBB-A7CF-B40F501FEA94}" name="values"/>
     <tableColumn id="3" xr3:uid="{65B84D6A-4F42-48EF-96C4-F96A9F83927A}" name="open"/>
     <tableColumn id="4" xr3:uid="{74E3F366-DDE3-4CFD-BA1C-66CEBEFAC6A8}" name="close"/>
@@ -366,6 +557,15 @@
     <tableColumn id="11" xr3:uid="{E1DE9D89-89DD-4951-8BF1-0176300F18D4}" name="slowPeriod"/>
     <tableColumn id="15" xr3:uid="{BC7489DE-CE64-46E7-968A-7C8570B46BF4}" name="signalPeriod"/>
     <tableColumn id="9" xr3:uid="{1E8FE46A-76A9-4653-87A3-3803850A4B11}" name="period"/>
+    <tableColumn id="14" xr3:uid="{C182A357-6815-4DEF-A7EB-DA640B5441F2}" name="noOfBars" dataDxfId="8"/>
+    <tableColumn id="23" xr3:uid="{41878FA0-F443-4DAD-B332-ACFAC9F243FE}" name="step" dataDxfId="0"/>
+    <tableColumn id="22" xr3:uid="{E6B7FD1A-101D-4CEA-B0DC-A79909D4CBAC}" name="max" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{708569BF-0118-40FC-9F0E-7833DE1C4BD5}" name="SimpleMAOscillator" dataDxfId="2"/>
+    <tableColumn id="20" xr3:uid="{945FA57F-9951-4198-BED1-B31D3FA516C3}" name="SimpleMASignal" dataDxfId="3"/>
+    <tableColumn id="19" xr3:uid="{F27568FA-17D6-4E44-89FB-D50D4746D5A0}" name="dPeriod" dataDxfId="4"/>
+    <tableColumn id="18" xr3:uid="{2C011B6E-4DEA-47EA-A41D-0DB6FA8437C7}" name="kPeriod" dataDxfId="5"/>
+    <tableColumn id="17" xr3:uid="{1907DA44-3698-4EA5-91E9-EA785D69114D}" name="rsiPeriod" dataDxfId="6"/>
+    <tableColumn id="16" xr3:uid="{8DE78FD6-16AB-4646-B519-FC591BC0B5C2}" name="stochasticPeriod" dataDxfId="7"/>
     <tableColumn id="13" xr3:uid="{641D8A5B-EB44-479F-89E4-CB18731A7447}" name="More"/>
     <tableColumn id="10" xr3:uid="{F9DD59E0-7B54-4023-B883-AAA574DC0D73}" name="result"/>
   </tableColumns>
@@ -670,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0F194F-9245-4289-9A12-8470106FF8A8}">
-  <dimension ref="A2:N28"/>
+  <dimension ref="A2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,97 +882,150 @@
     <col min="2" max="8" width="11.109375" customWidth="1"/>
     <col min="9" max="11" width="13.5546875" customWidth="1"/>
     <col min="12" max="12" width="11.109375" customWidth="1"/>
-    <col min="13" max="13" width="85.21875" customWidth="1"/>
-    <col min="14" max="14" width="63" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
+    <col min="15" max="15" width="9" customWidth="1"/>
+    <col min="16" max="16" width="22" customWidth="1"/>
+    <col min="17" max="17" width="18.77734375" customWidth="1"/>
+    <col min="18" max="19" width="11.109375" customWidth="1"/>
+    <col min="20" max="20" width="12.33203125" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" customWidth="1"/>
+    <col min="22" max="22" width="90.33203125" customWidth="1"/>
+    <col min="23" max="23" width="63" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:23" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="W3" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="1"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="8"/>
-      <c r="N4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -786,219 +1039,314 @@
       <c r="K5" s="1"/>
       <c r="L5" s="4"/>
       <c r="M5" s="8"/>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
+      <c r="W5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="4"/>
       <c r="M6" s="8"/>
-      <c r="N6" t="s">
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="4"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="4"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="1"/>
       <c r="M7" s="8"/>
-      <c r="N7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="H8" s="4"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="4"/>
       <c r="M8" s="8"/>
-      <c r="N8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="4"/>
       <c r="M9" s="8"/>
-      <c r="N9" s="7" t="s">
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="N10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K10" s="1"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="4"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="1"/>
-      <c r="N11" t="s">
+      <c r="K11" s="4"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="1"/>
+      <c r="W12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="4"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="4"/>
+      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="1"/>
+      <c r="W13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="1"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="4"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N14" t="s">
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="1"/>
+      <c r="W14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="4"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="1"/>
-      <c r="N15" t="s">
+      <c r="L15" s="1"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="1"/>
+      <c r="W15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="1"/>
@@ -1011,14 +1359,23 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="1"/>
-      <c r="N16" t="s">
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="1"/>
+      <c r="W16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="1"/>
@@ -1031,56 +1388,81 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="4"/>
-      <c r="M17" s="1"/>
-      <c r="N17" t="s">
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="1"/>
+      <c r="W17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="1"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="4"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="4"/>
+      <c r="K18" s="1"/>
       <c r="L18" s="4"/>
-      <c r="M18" s="1"/>
-      <c r="N18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="1"/>
+      <c r="W18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="N19" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="1"/>
+      <c r="W19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="1"/>
@@ -1092,97 +1474,140 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="1"/>
-      <c r="N20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L20" s="9"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="4"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" t="s">
+      <c r="L21" s="4"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="1"/>
+      <c r="W21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1"/>
-      <c r="C22" s="4"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" t="s">
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="1"/>
+      <c r="W22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="12"/>
+      <c r="G23" s="4"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
-      <c r="M23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N23" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="1"/>
+      <c r="W23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="12"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="1"/>
-      <c r="N24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L24" s="1"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="1"/>
+      <c r="W24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="1"/>
@@ -1195,17 +1620,26 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="4"/>
-      <c r="M25" s="1"/>
-      <c r="N25" t="s">
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="1"/>
+      <c r="W25" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="4"/>
-      <c r="C26" s="9"/>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -1215,38 +1649,56 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="1"/>
-      <c r="N26" t="s">
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="1"/>
+      <c r="W26" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="1"/>
-      <c r="N27" t="s">
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8"/>
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8"/>
+      <c r="V27" s="1"/>
+      <c r="W27" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="9"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
+      <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="1"/>
@@ -1254,42 +1706,96 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N28" s="6" t="s">
-        <v>53</v>
-      </c>
+      <c r="L28" s="4"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="1"/>
+      <c r="W28" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W29" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="M32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="J35" s="7"/>
+    </row>
+    <row r="42" spans="10:22" x14ac:dyDescent="0.3">
+      <c r="V42" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="H2:U2"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" tooltip="ADL" display="https://tonicdev.com/anandaravindan/adl" xr:uid="{25F67245-1C75-403D-8D33-DC61ACD919FF}"/>
-    <hyperlink ref="A4" r:id="rId2" tooltip="ADX" display="https://github.com/anandanand84/technicalindicators/blob/master/test/directionalmovement/ADX.js" xr:uid="{FF1693AA-6202-4B93-9C09-BA4041CDDD9C}"/>
-    <hyperlink ref="A5" r:id="rId3" tooltip="ATR" display="https://tonicdev.com/anandaravindan/atr" xr:uid="{2B10D00F-6D1E-4232-86AA-83332A06993B}"/>
-    <hyperlink ref="A6" r:id="rId4" tooltip="AO" display="https://github.com/anandanand84/technicalindicators/blob/master/test/oscillators/AwesomeOscillator.js" xr:uid="{B01181A2-DE71-4DA1-878F-05F43881BC42}"/>
-    <hyperlink ref="A7" r:id="rId5" tooltip="BB" display="https://tonicdev.com/anandaravindan/bb" xr:uid="{F0117AB1-F63F-46EB-956A-A26837D80336}"/>
-    <hyperlink ref="A8" r:id="rId6" tooltip="CCI" display="https://github.com/anandanand84/technicalindicators/blob/master/test/oscillators/CCI.js" xr:uid="{9740AAD8-602A-4ECD-B6C7-112F453B0A1A}"/>
-    <hyperlink ref="A9" r:id="rId7" tooltip="FI" display="https://github.com/anandanand84/technicalindicators/blob/master/test/volume/ForceIndex.js" xr:uid="{EBE91B90-5F01-4C46-99DC-5CF949A9BBC1}"/>
-    <hyperlink ref="A10" r:id="rId8" tooltip="KST" display="https://tonicdev.com/anandaravindan/kst" xr:uid="{CBEB55C9-AE62-4262-A209-7A31F4AA1FDC}"/>
-    <hyperlink ref="A11" r:id="rId9" tooltip="MFI" display="https://github.com/anandanand84/technicalindicators/blob/master/test/volume/MFI.js" xr:uid="{4A08186C-5D9F-4655-9D32-B67A8B6B476F}"/>
-    <hyperlink ref="A12" r:id="rId10" tooltip="MACD" display="https://tonicdev.com/anandaravindan/macd" xr:uid="{097BB385-67F2-457C-9DDC-33E25CFFAAB2}"/>
-    <hyperlink ref="A13" r:id="rId11" tooltip="OBV" display="https://tonicdev.com/anandaravindan/obv" xr:uid="{3F959E21-7A0B-4A02-80C4-832CB5AC7247}"/>
-    <hyperlink ref="A14" r:id="rId12" tooltip="PSAR" display="https://github.com/anandanand84/technicalindicators/blob/master/test/momentum/PSAR.js" xr:uid="{3A3E88C4-81BB-4804-9603-71D0F28363F8}"/>
-    <hyperlink ref="A15" r:id="rId13" tooltip="ROC" display="https://tonicdev.com/anandaravindan/roc" xr:uid="{6FE572CD-B185-4711-8AD0-C0A21AE8FF3C}"/>
-    <hyperlink ref="A16" r:id="rId14" tooltip="RSI" display="https://tonicdev.com/anandaravindan/rsi" xr:uid="{F0165D2F-0CAE-48C4-825B-59F166095635}"/>
-    <hyperlink ref="A17" r:id="rId15" tooltip="SMA" display="https://tonicdev.com/anandaravindan/sma" xr:uid="{2D7E7DB3-D5F9-48FA-AC6A-BCE720B87398}"/>
-    <hyperlink ref="A18" r:id="rId16" tooltip="KD" display="https://tonicdev.com/anandaravindan/stochastic" xr:uid="{F80EACED-F045-4099-80C9-4B92CA46E7DE}"/>
-    <hyperlink ref="A19" r:id="rId17" tooltip="StochRSI" display="https://tonicdev.com/anandaravindan/stochasticrsi" xr:uid="{3FAE60C1-E971-41B3-9B4D-4EA392B08320}"/>
-    <hyperlink ref="A20" r:id="rId18" tooltip="TRIX" display="https://tonicdev.com/anandaravindan/trix" xr:uid="{21D4ACCB-048F-417D-82E1-68B67F2CA253}"/>
-    <hyperlink ref="A21" r:id="rId19" tooltip="Typical Price" display="https://github.com/anandanand84/technicalindicators/blob/master/test/chart_types/TypicalPrice.js" xr:uid="{538888FC-5588-4299-B9F2-3FA455AEDABA}"/>
-    <hyperlink ref="A22" r:id="rId20" tooltip="VWAP" display="https://github.com/anandanand84/technicalindicators/blob/master/test/volume/VWAP.js" xr:uid="{B36EF0CA-5C24-4283-AB06-745B244D4C95}"/>
-    <hyperlink ref="A23" r:id="rId21" tooltip="VP" display="https://github.com/anandanand84/technicalindicators/blob/master/test/volume/VolumeProfile.js" xr:uid="{3B15637A-A2C0-410D-9F57-9209F0C17424}"/>
-    <hyperlink ref="A24" r:id="rId22" tooltip="EMA" display="https://tonicdev.com/anandaravindan/ema" xr:uid="{E83E7423-5A74-4AB7-8B02-F9AAE335C3E1}"/>
-    <hyperlink ref="A25" r:id="rId23" tooltip="WMA" display="https://tonicdev.com/anandaravindan/wma" xr:uid="{FC0051EF-BA81-4C98-9EE3-50D976C89A0F}"/>
-    <hyperlink ref="A26" r:id="rId24" tooltip="WEMA" display="https://tonicdev.com/anandaravindan/wema" xr:uid="{028E2EF5-86C8-4015-AB67-68615C1D6E42}"/>
-    <hyperlink ref="A27" r:id="rId25" tooltip="W%R" display="https://tonicdev.com/anandaravindan/williamsr" xr:uid="{78C3A0BF-0BD9-4702-9C51-20FC31CB0B53}"/>
-    <hyperlink ref="A28" r:id="rId26" tooltip="Ichimoku Cloud" display="https://github.com/anandanand84/technicalindicators/blob/master/test/ichimoku/IchimokuCloud.js" xr:uid="{8EF2ACF9-89D6-4854-9F6A-212D881FA18D}"/>
+    <hyperlink ref="A4" r:id="rId1" tooltip="ADL" display="https://tonicdev.com/anandaravindan/adl" xr:uid="{25F67245-1C75-403D-8D33-DC61ACD919FF}"/>
+    <hyperlink ref="A5" r:id="rId2" tooltip="ADX" display="https://github.com/anandanand84/technicalindicators/blob/master/test/directionalmovement/ADX.js" xr:uid="{FF1693AA-6202-4B93-9C09-BA4041CDDD9C}"/>
+    <hyperlink ref="A6" r:id="rId3" tooltip="ATR" display="https://tonicdev.com/anandaravindan/atr" xr:uid="{2B10D00F-6D1E-4232-86AA-83332A06993B}"/>
+    <hyperlink ref="A7" r:id="rId4" tooltip="AO" display="https://github.com/anandanand84/technicalindicators/blob/master/test/oscillators/AwesomeOscillator.js" xr:uid="{B01181A2-DE71-4DA1-878F-05F43881BC42}"/>
+    <hyperlink ref="A8" r:id="rId5" tooltip="BB" display="https://tonicdev.com/anandaravindan/bb" xr:uid="{F0117AB1-F63F-46EB-956A-A26837D80336}"/>
+    <hyperlink ref="A9" r:id="rId6" tooltip="CCI" display="https://github.com/anandanand84/technicalindicators/blob/master/test/oscillators/CCI.js" xr:uid="{9740AAD8-602A-4ECD-B6C7-112F453B0A1A}"/>
+    <hyperlink ref="A10" r:id="rId7" tooltip="FI" display="https://github.com/anandanand84/technicalindicators/blob/master/test/volume/ForceIndex.js" xr:uid="{EBE91B90-5F01-4C46-99DC-5CF949A9BBC1}"/>
+    <hyperlink ref="A11" r:id="rId8" tooltip="KST" display="https://tonicdev.com/anandaravindan/kst" xr:uid="{CBEB55C9-AE62-4262-A209-7A31F4AA1FDC}"/>
+    <hyperlink ref="A12" r:id="rId9" tooltip="MFI" display="https://github.com/anandanand84/technicalindicators/blob/master/test/volume/MFI.js" xr:uid="{4A08186C-5D9F-4655-9D32-B67A8B6B476F}"/>
+    <hyperlink ref="A13" r:id="rId10" tooltip="MACD" display="https://tonicdev.com/anandaravindan/macd" xr:uid="{097BB385-67F2-457C-9DDC-33E25CFFAAB2}"/>
+    <hyperlink ref="A14" r:id="rId11" tooltip="OBV" display="https://tonicdev.com/anandaravindan/obv" xr:uid="{3F959E21-7A0B-4A02-80C4-832CB5AC7247}"/>
+    <hyperlink ref="A15" r:id="rId12" tooltip="PSAR" display="https://github.com/anandanand84/technicalindicators/blob/master/test/momentum/PSAR.js" xr:uid="{3A3E88C4-81BB-4804-9603-71D0F28363F8}"/>
+    <hyperlink ref="A16" r:id="rId13" tooltip="ROC" display="https://tonicdev.com/anandaravindan/roc" xr:uid="{6FE572CD-B185-4711-8AD0-C0A21AE8FF3C}"/>
+    <hyperlink ref="A17" r:id="rId14" tooltip="RSI" display="https://tonicdev.com/anandaravindan/rsi" xr:uid="{F0165D2F-0CAE-48C4-825B-59F166095635}"/>
+    <hyperlink ref="A18" r:id="rId15" tooltip="SMA" display="https://tonicdev.com/anandaravindan/sma" xr:uid="{2D7E7DB3-D5F9-48FA-AC6A-BCE720B87398}"/>
+    <hyperlink ref="A19" r:id="rId16" tooltip="KD" display="https://tonicdev.com/anandaravindan/stochastic" xr:uid="{F80EACED-F045-4099-80C9-4B92CA46E7DE}"/>
+    <hyperlink ref="A20" r:id="rId17" tooltip="StochRSI" display="https://tonicdev.com/anandaravindan/stochasticrsi" xr:uid="{3FAE60C1-E971-41B3-9B4D-4EA392B08320}"/>
+    <hyperlink ref="A21" r:id="rId18" tooltip="TRIX" display="https://tonicdev.com/anandaravindan/trix" xr:uid="{21D4ACCB-048F-417D-82E1-68B67F2CA253}"/>
+    <hyperlink ref="A22" r:id="rId19" tooltip="Typical Price" display="https://github.com/anandanand84/technicalindicators/blob/master/test/chart_types/TypicalPrice.js" xr:uid="{538888FC-5588-4299-B9F2-3FA455AEDABA}"/>
+    <hyperlink ref="A23" r:id="rId20" tooltip="VWAP" display="https://github.com/anandanand84/technicalindicators/blob/master/test/volume/VWAP.js" xr:uid="{B36EF0CA-5C24-4283-AB06-745B244D4C95}"/>
+    <hyperlink ref="A24" r:id="rId21" tooltip="VP" display="https://github.com/anandanand84/technicalindicators/blob/master/test/volume/VolumeProfile.js" xr:uid="{3B15637A-A2C0-410D-9F57-9209F0C17424}"/>
+    <hyperlink ref="A25" r:id="rId22" tooltip="EMA" display="https://tonicdev.com/anandaravindan/ema" xr:uid="{E83E7423-5A74-4AB7-8B02-F9AAE335C3E1}"/>
+    <hyperlink ref="A26" r:id="rId23" tooltip="WMA" display="https://tonicdev.com/anandaravindan/wma" xr:uid="{FC0051EF-BA81-4C98-9EE3-50D976C89A0F}"/>
+    <hyperlink ref="A27" r:id="rId24" tooltip="WEMA" display="https://tonicdev.com/anandaravindan/wema" xr:uid="{028E2EF5-86C8-4015-AB67-68615C1D6E42}"/>
+    <hyperlink ref="A28" r:id="rId25" tooltip="W%R" display="https://tonicdev.com/anandaravindan/williamsr" xr:uid="{78C3A0BF-0BD9-4702-9C51-20FC31CB0B53}"/>
+    <hyperlink ref="A29" r:id="rId26" tooltip="Ichimoku Cloud" display="https://github.com/anandanand84/technicalindicators/blob/master/test/ichimoku/IchimokuCloud.js" xr:uid="{8EF2ACF9-89D6-4854-9F6A-212D881FA18D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
@@ -1300,6 +1806,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011ECEEA5ABD33947B365210533CD1308" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf585822e3b881e90487c487a90d9785">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="186b77a3-44ba-43ea-a47d-48e0bb758210" xmlns:ns4="7c8f8b64-a5df-46c4-8af9-77684a301d74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a1408beef0212d2fd1d87b0b35ce6ff" ns3:_="" ns4:_="">
     <xsd:import namespace="186b77a3-44ba-43ea-a47d-48e0bb758210"/>
@@ -1490,15 +2005,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1506,6 +2012,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA8916DF-E5C6-46E0-B100-470C99F6DD56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55122CB5-F2B1-4C22-9641-6937C3CBFF32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1520,14 +2034,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA8916DF-E5C6-46E0-B100-470C99F6DD56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added technical indicator default values and more config
</commit_message>
<xml_diff>
--- a/server/technical-indicators-info.xlsx
+++ b/server/technical-indicators-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bb5771db89f4b71/Desktop/UNI/Fourth year/Dissertation/Repo/ATPlatform/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{40C82BBD-ECCF-4B81-8A0C-E8C14A058AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D0AC1AC1-2CF4-4418-ACD1-8B1B96A80AAC}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="8_{40C82BBD-ECCF-4B81-8A0C-E8C14A058AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{937014DC-3D9C-4589-A1FA-087FC1CEF3A1}"/>
   <bookViews>
-    <workbookView xWindow="13308" yWindow="3240" windowWidth="14352" windowHeight="11328" xr2:uid="{07D8F586-ED62-4F25-AB07-0DF1C28F4F51}"/>
+    <workbookView xWindow="8688" yWindow="1032" windowWidth="14352" windowHeight="11328" xr2:uid="{07D8F586-ED62-4F25-AB07-0DF1C28F4F51}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -400,6 +400,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -407,9 +410,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -558,14 +558,14 @@
     <tableColumn id="15" xr3:uid="{BC7489DE-CE64-46E7-968A-7C8570B46BF4}" name="signalPeriod"/>
     <tableColumn id="9" xr3:uid="{1E8FE46A-76A9-4653-87A3-3803850A4B11}" name="period"/>
     <tableColumn id="14" xr3:uid="{C182A357-6815-4DEF-A7EB-DA640B5441F2}" name="noOfBars" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{41878FA0-F443-4DAD-B332-ACFAC9F243FE}" name="step" dataDxfId="0"/>
-    <tableColumn id="22" xr3:uid="{E6B7FD1A-101D-4CEA-B0DC-A79909D4CBAC}" name="max" dataDxfId="1"/>
-    <tableColumn id="21" xr3:uid="{708569BF-0118-40FC-9F0E-7833DE1C4BD5}" name="SimpleMAOscillator" dataDxfId="2"/>
-    <tableColumn id="20" xr3:uid="{945FA57F-9951-4198-BED1-B31D3FA516C3}" name="SimpleMASignal" dataDxfId="3"/>
-    <tableColumn id="19" xr3:uid="{F27568FA-17D6-4E44-89FB-D50D4746D5A0}" name="dPeriod" dataDxfId="4"/>
-    <tableColumn id="18" xr3:uid="{2C011B6E-4DEA-47EA-A41D-0DB6FA8437C7}" name="kPeriod" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{1907DA44-3698-4EA5-91E9-EA785D69114D}" name="rsiPeriod" dataDxfId="6"/>
-    <tableColumn id="16" xr3:uid="{8DE78FD6-16AB-4646-B519-FC591BC0B5C2}" name="stochasticPeriod" dataDxfId="7"/>
+    <tableColumn id="23" xr3:uid="{41878FA0-F443-4DAD-B332-ACFAC9F243FE}" name="step" dataDxfId="7"/>
+    <tableColumn id="22" xr3:uid="{E6B7FD1A-101D-4CEA-B0DC-A79909D4CBAC}" name="max" dataDxfId="6"/>
+    <tableColumn id="21" xr3:uid="{708569BF-0118-40FC-9F0E-7833DE1C4BD5}" name="SimpleMAOscillator" dataDxfId="5"/>
+    <tableColumn id="20" xr3:uid="{945FA57F-9951-4198-BED1-B31D3FA516C3}" name="SimpleMASignal" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{F27568FA-17D6-4E44-89FB-D50D4746D5A0}" name="dPeriod" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{2C011B6E-4DEA-47EA-A41D-0DB6FA8437C7}" name="kPeriod" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{1907DA44-3698-4EA5-91E9-EA785D69114D}" name="rsiPeriod" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{8DE78FD6-16AB-4646-B519-FC591BC0B5C2}" name="stochasticPeriod" dataDxfId="0"/>
     <tableColumn id="13" xr3:uid="{641D8A5B-EB44-479F-89E4-CB18731A7447}" name="More"/>
     <tableColumn id="10" xr3:uid="{F9DD59E0-7B54-4023-B883-AAA574DC0D73}" name="result"/>
   </tableColumns>
@@ -872,14 +872,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0F194F-9245-4289-9A12-8470106FF8A8}">
   <dimension ref="A2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54.44140625" style="11" customWidth="1"/>
-    <col min="2" max="8" width="11.109375" customWidth="1"/>
+    <col min="2" max="7" width="11.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" customWidth="1"/>
     <col min="9" max="11" width="13.5546875" customWidth="1"/>
     <col min="12" max="12" width="11.109375" customWidth="1"/>
     <col min="13" max="13" width="12.88671875" customWidth="1"/>
@@ -896,30 +897,30 @@
   <sheetData>
     <row r="2" spans="1:23" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="16" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="19"/>
       <c r="V2" s="14"/>
       <c r="W2" s="14"/>
     </row>
@@ -1037,7 +1038,9 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="4"/>
+      <c r="L5" s="4">
+        <v>14</v>
+      </c>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
@@ -1066,7 +1069,9 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="4"/>
+      <c r="L6" s="4">
+        <v>14</v>
+      </c>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
@@ -1092,8 +1097,12 @@
       <c r="F7" s="4"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="I7" s="4">
+        <v>5</v>
+      </c>
+      <c r="J7" s="4">
+        <v>34</v>
+      </c>
       <c r="K7" s="8"/>
       <c r="L7" s="1"/>
       <c r="M7" s="8"/>
@@ -1180,7 +1189,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="J10" s="9"/>
       <c r="K10" s="1"/>
       <c r="L10" s="4"/>
       <c r="M10" s="8"/>
@@ -1806,15 +1815,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011ECEEA5ABD33947B365210533CD1308" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf585822e3b881e90487c487a90d9785">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="186b77a3-44ba-43ea-a47d-48e0bb758210" xmlns:ns4="7c8f8b64-a5df-46c4-8af9-77684a301d74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a1408beef0212d2fd1d87b0b35ce6ff" ns3:_="" ns4:_="">
     <xsd:import namespace="186b77a3-44ba-43ea-a47d-48e0bb758210"/>
@@ -2005,6 +2005,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2012,14 +2021,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA8916DF-E5C6-46E0-B100-470C99F6DD56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55122CB5-F2B1-4C22-9641-6937C3CBFF32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2034,6 +2035,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA8916DF-E5C6-46E0-B100-470C99F6DD56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
cron strategy dev, other changes
</commit_message>
<xml_diff>
--- a/server/technical-indicators-info.xlsx
+++ b/server/technical-indicators-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bb5771db89f4b71/Desktop/UNI/Fourth year/Dissertation/Repo/ATPlatform/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{40C82BBD-ECCF-4B81-8A0C-E8C14A058AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{937014DC-3D9C-4589-A1FA-087FC1CEF3A1}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{40C82BBD-ECCF-4B81-8A0C-E8C14A058AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6CB421E2-33DF-4ADF-8E55-33F7C140E63D}"/>
   <bookViews>
-    <workbookView xWindow="8688" yWindow="1032" windowWidth="14352" windowHeight="11328" xr2:uid="{07D8F586-ED62-4F25-AB07-0DF1C28F4F51}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07D8F586-ED62-4F25-AB07-0DF1C28F4F51}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -276,7 +276,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +304,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF4747"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
@@ -411,6 +423,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -530,6 +548,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF4747"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -872,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0F194F-9245-4289-9A12-8470106FF8A8}">
   <dimension ref="A2:W42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -996,7 +1019,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
@@ -1025,7 +1048,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="21" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
@@ -1815,6 +1838,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011ECEEA5ABD33947B365210533CD1308" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf585822e3b881e90487c487a90d9785">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="186b77a3-44ba-43ea-a47d-48e0bb758210" xmlns:ns4="7c8f8b64-a5df-46c4-8af9-77684a301d74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a1408beef0212d2fd1d87b0b35ce6ff" ns3:_="" ns4:_="">
     <xsd:import namespace="186b77a3-44ba-43ea-a47d-48e0bb758210"/>
@@ -2005,15 +2037,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2021,6 +2044,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA8916DF-E5C6-46E0-B100-470C99F6DD56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55122CB5-F2B1-4C22-9641-6937C3CBFF32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2035,14 +2066,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA8916DF-E5C6-46E0-B100-470C99F6DD56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
removed signalConfig, added signals creation support with indicators components, more refactoring
</commit_message>
<xml_diff>
--- a/server/technical-indicators-info.xlsx
+++ b/server/technical-indicators-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bb5771db89f4b71/Desktop/UNI/Fourth year/Dissertation/Repo/ATPlatform/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="106" documentId="8_{40C82BBD-ECCF-4B81-8A0C-E8C14A058AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6CB421E2-33DF-4ADF-8E55-33F7C140E63D}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{40C82BBD-ECCF-4B81-8A0C-E8C14A058AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2940A270-0246-40EC-B861-8506D91F35AC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{07D8F586-ED62-4F25-AB07-0DF1C28F4F51}"/>
+    <workbookView xWindow="16995" yWindow="-12135" windowWidth="21600" windowHeight="11325" xr2:uid="{07D8F586-ED62-4F25-AB07-0DF1C28F4F51}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -412,6 +412,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -423,12 +429,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -902,48 +902,47 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54.44140625" style="11" customWidth="1"/>
-    <col min="2" max="7" width="11.109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" customWidth="1"/>
-    <col min="9" max="11" width="13.5546875" customWidth="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" customWidth="1"/>
-    <col min="15" max="15" width="9" customWidth="1"/>
-    <col min="16" max="16" width="22" customWidth="1"/>
-    <col min="17" max="17" width="18.77734375" customWidth="1"/>
-    <col min="18" max="19" width="11.109375" customWidth="1"/>
-    <col min="20" max="20" width="12.33203125" customWidth="1"/>
-    <col min="21" max="21" width="19.44140625" customWidth="1"/>
-    <col min="22" max="22" width="90.33203125" customWidth="1"/>
+    <col min="2" max="8" width="11.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="11" width="13.5546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="9" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="22" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="18.77734375" hidden="1" customWidth="1"/>
+    <col min="18" max="19" width="11.109375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="12.33203125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="19.44140625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="90.33203125" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="36.6" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="18"/>
-      <c r="T2" s="18"/>
-      <c r="U2" s="19"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="21"/>
       <c r="V2" s="14"/>
       <c r="W2" s="14"/>
     </row>
@@ -1019,7 +1018,7 @@
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="16" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1"/>
@@ -1048,7 +1047,7 @@
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
@@ -1838,15 +1837,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010011ECEEA5ABD33947B365210533CD1308" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cf585822e3b881e90487c487a90d9785">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="186b77a3-44ba-43ea-a47d-48e0bb758210" xmlns:ns4="7c8f8b64-a5df-46c4-8af9-77684a301d74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a1408beef0212d2fd1d87b0b35ce6ff" ns3:_="" ns4:_="">
     <xsd:import namespace="186b77a3-44ba-43ea-a47d-48e0bb758210"/>
@@ -2037,6 +2027,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2044,14 +2043,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA8916DF-E5C6-46E0-B100-470C99F6DD56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55122CB5-F2B1-4C22-9641-6937C3CBFF32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2066,6 +2057,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA8916DF-E5C6-46E0-B100-470C99F6DD56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>